<commit_message>
Update high school data from Grokipedia (all teams)
- Scraped remaining 14 teams via Grokipedia
- Total high schools: 121 (was 65 from Wikipedia alone)
- Added 56 new high schools from Grokipedia
- Cleaned up 4 incorrectly extracted entries
- Updated Excel exports with latest data

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/major_league_soccer_rosters.xlsx
+++ b/output/major_league_soccer_rosters.xlsx
@@ -10564,11 +10564,31 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H138" t="inlineStr"/>
-      <c r="I138" t="inlineStr"/>
-      <c r="J138" t="inlineStr"/>
-      <c r="K138" t="inlineStr"/>
-      <c r="L138" t="inlineStr"/>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Chatfield High School</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>Littleton</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>Colorado</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Cole_Bassett</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M138" t="inlineStr">
         <is>
           <t>Midfielder</t>
@@ -10603,7 +10623,7 @@
       </c>
       <c r="W138" t="inlineStr">
         <is>
-          <t>2026-01-28T03:01:44.922545</t>
+          <t>2026-01-28 23:49:20</t>
         </is>
       </c>
     </row>
@@ -14839,11 +14859,31 @@
           <t>Senegal</t>
         </is>
       </c>
-      <c r="H195" t="inlineStr"/>
-      <c r="I195" t="inlineStr"/>
-      <c r="J195" t="inlineStr"/>
-      <c r="K195" t="inlineStr"/>
-      <c r="L195" t="inlineStr"/>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>Episcopal High School</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>Alexandria</t>
+        </is>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Dominique_Badji</t>
+        </is>
+      </c>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M195" t="inlineStr">
         <is>
           <t>Forward</t>
@@ -14878,7 +14918,7 @@
       </c>
       <c r="W195" t="inlineStr">
         <is>
-          <t>2026-01-28T03:12:41.223028</t>
+          <t>2026-01-28 23:06:19</t>
         </is>
       </c>
     </row>
@@ -14989,11 +15029,31 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H197" t="inlineStr"/>
-      <c r="I197" t="inlineStr"/>
-      <c r="J197" t="inlineStr"/>
-      <c r="K197" t="inlineStr"/>
-      <c r="L197" t="inlineStr"/>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>St. Thomas Aquinas High School</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>Overland Park</t>
+        </is>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>Kansas</t>
+        </is>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Lucas_Bartlett</t>
+        </is>
+      </c>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M197" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -15028,7 +15088,7 @@
       </c>
       <c r="W197" t="inlineStr">
         <is>
-          <t>2026-01-28T03:10:39.591369</t>
+          <t>2026-01-28 23:06:39</t>
         </is>
       </c>
     </row>
@@ -15684,11 +15744,31 @@
           <t>Japan</t>
         </is>
       </c>
-      <c r="H206" t="inlineStr"/>
-      <c r="I206" t="inlineStr"/>
-      <c r="J206" t="inlineStr"/>
-      <c r="K206" t="inlineStr"/>
-      <c r="L206" t="inlineStr"/>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>Osaka Toin High School</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>Daito</t>
+        </is>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>Osaka</t>
+        </is>
+      </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/keisuke_kurokawa</t>
+        </is>
+      </c>
+      <c r="L206" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M206" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -15723,7 +15803,7 @@
       </c>
       <c r="W206" t="inlineStr">
         <is>
-          <t>2026-01-28T03:11:29.487044</t>
+          <t>2026-01-28 23:08:08</t>
         </is>
       </c>
     </row>
@@ -15871,7 +15951,7 @@
       </c>
       <c r="W208" t="inlineStr">
         <is>
-          <t>2026-01-28 11:09:59</t>
+          <t>2026-01-28 23:08:28</t>
         </is>
       </c>
     </row>
@@ -15907,11 +15987,31 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H209" t="inlineStr"/>
-      <c r="I209" t="inlineStr"/>
-      <c r="J209" t="inlineStr"/>
-      <c r="K209" t="inlineStr"/>
-      <c r="L209" t="inlineStr"/>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>Massapequa High School</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>Massapequa</t>
+        </is>
+      </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Sean_Nealis</t>
+        </is>
+      </c>
+      <c r="L209" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M209" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -15946,7 +16046,7 @@
       </c>
       <c r="W209" t="inlineStr">
         <is>
-          <t>2026-01-28T03:11:45.972234</t>
+          <t>2026-01-28 23:08:38</t>
         </is>
       </c>
     </row>
@@ -16205,11 +16305,23 @@
           <t>Australia</t>
         </is>
       </c>
-      <c r="H213" t="inlineStr"/>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>Palm Beach Currumbin State High School</t>
+        </is>
+      </c>
       <c r="I213" t="inlineStr"/>
       <c r="J213" t="inlineStr"/>
-      <c r="K213" t="inlineStr"/>
-      <c r="L213" t="inlineStr"/>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Kye_Rowles</t>
+        </is>
+      </c>
+      <c r="L213" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M213" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -16244,7 +16356,7 @@
       </c>
       <c r="W213" t="inlineStr">
         <is>
-          <t>2026-01-28T03:12:08.044106</t>
+          <t>2026-01-28 23:09:23</t>
         </is>
       </c>
     </row>
@@ -16430,11 +16542,23 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H216" t="inlineStr"/>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>Seton Hall Prep</t>
+        </is>
+      </c>
       <c r="I216" t="inlineStr"/>
       <c r="J216" t="inlineStr"/>
-      <c r="K216" t="inlineStr"/>
-      <c r="L216" t="inlineStr"/>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Jared_Stroud</t>
+        </is>
+      </c>
+      <c r="L216" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M216" t="inlineStr">
         <is>
           <t>Midfielder</t>
@@ -16469,7 +16593,7 @@
       </c>
       <c r="W216" t="inlineStr">
         <is>
-          <t>2026-01-28T03:12:24.552154</t>
+          <t>2026-01-28 23:10:03</t>
         </is>
       </c>
     </row>
@@ -17312,11 +17436,23 @@
           <t>Zimbabwe</t>
         </is>
       </c>
-      <c r="H228" t="inlineStr"/>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>Mzilikazi High School</t>
+        </is>
+      </c>
       <c r="I228" t="inlineStr"/>
       <c r="J228" t="inlineStr"/>
-      <c r="K228" t="inlineStr"/>
-      <c r="L228" t="inlineStr"/>
+      <c r="K228" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Teenage_Hadebe</t>
+        </is>
+      </c>
+      <c r="L228" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M228" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -17351,7 +17487,7 @@
       </c>
       <c r="W228" t="inlineStr">
         <is>
-          <t>2026-01-28T02:59:21.267227</t>
+          <t>2026-01-29 00:02:34</t>
         </is>
       </c>
     </row>
@@ -17713,11 +17849,23 @@
           <t>Sierra Leone</t>
         </is>
       </c>
-      <c r="H233" t="inlineStr"/>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>Leuzinger High School</t>
+        </is>
+      </c>
       <c r="I233" t="inlineStr"/>
       <c r="J233" t="inlineStr"/>
-      <c r="K233" t="inlineStr"/>
-      <c r="L233" t="inlineStr"/>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Kei_Kamara</t>
+        </is>
+      </c>
+      <c r="L233" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M233" t="inlineStr">
         <is>
           <t>Forward</t>
@@ -17752,7 +17900,7 @@
       </c>
       <c r="W233" t="inlineStr">
         <is>
-          <t>2026-01-28T03:00:46.308909</t>
+          <t>2026-01-29 00:03:08</t>
         </is>
       </c>
     </row>
@@ -18276,11 +18424,23 @@
           <t>Jamaica</t>
         </is>
       </c>
-      <c r="H240" t="inlineStr"/>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>Paul Bogle High School</t>
+        </is>
+      </c>
       <c r="I240" t="inlineStr"/>
       <c r="J240" t="inlineStr"/>
-      <c r="K240" t="inlineStr"/>
-      <c r="L240" t="inlineStr"/>
+      <c r="K240" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Alvas_Powell</t>
+        </is>
+      </c>
+      <c r="L240" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M240" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -18315,7 +18475,7 @@
       </c>
       <c r="W240" t="inlineStr">
         <is>
-          <t>2026-01-28T03:00:15.240469</t>
+          <t>2026-01-29 00:03:58</t>
         </is>
       </c>
     </row>
@@ -18663,11 +18823,23 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H245" t="inlineStr"/>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>Boca Raton Community High School</t>
+        </is>
+      </c>
       <c r="I245" t="inlineStr"/>
       <c r="J245" t="inlineStr"/>
-      <c r="K245" t="inlineStr"/>
-      <c r="L245" t="inlineStr"/>
+      <c r="K245" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/gerardo_valenzuela</t>
+        </is>
+      </c>
+      <c r="L245" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M245" t="inlineStr">
         <is>
           <t>Midfielder</t>
@@ -18700,7 +18872,7 @@
       </c>
       <c r="W245" t="inlineStr">
         <is>
-          <t>2026-01-28T03:00:39.892884</t>
+          <t>2026-01-29 00:04:47</t>
         </is>
       </c>
     </row>
@@ -21148,11 +21320,23 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H278" t="inlineStr"/>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>Evergreen High School</t>
+        </is>
+      </c>
       <c r="I278" t="inlineStr"/>
       <c r="J278" t="inlineStr"/>
-      <c r="K278" t="inlineStr"/>
-      <c r="L278" t="inlineStr"/>
+      <c r="K278" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Griffin_Dorsey</t>
+        </is>
+      </c>
+      <c r="L278" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M278" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -21187,7 +21371,7 @@
       </c>
       <c r="W278" t="inlineStr">
         <is>
-          <t>2026-01-28T03:13:16.103485</t>
+          <t>2026-01-28 23:21:15</t>
         </is>
       </c>
     </row>
@@ -31024,23 +31208,11 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H408" t="inlineStr">
-        <is>
-          <t>Lake Highlands Junior High School</t>
-        </is>
-      </c>
+      <c r="H408" t="inlineStr"/>
       <c r="I408" t="inlineStr"/>
       <c r="J408" t="inlineStr"/>
-      <c r="K408" t="inlineStr">
-        <is>
-          <t>https://grokipedia.com/page/matthew_corcoran</t>
-        </is>
-      </c>
-      <c r="L408" t="inlineStr">
-        <is>
-          <t>Grokipedia</t>
-        </is>
-      </c>
+      <c r="K408" t="inlineStr"/>
+      <c r="L408" t="inlineStr"/>
       <c r="M408" t="inlineStr">
         <is>
           <t>Midfielder</t>
@@ -42669,11 +42841,23 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H569" t="inlineStr"/>
+      <c r="H569" t="inlineStr">
+        <is>
+          <t>Portage Northern High School</t>
+        </is>
+      </c>
       <c r="I569" t="inlineStr"/>
       <c r="J569" t="inlineStr"/>
-      <c r="K569" t="inlineStr"/>
-      <c r="L569" t="inlineStr"/>
+      <c r="K569" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/brandon_bye</t>
+        </is>
+      </c>
+      <c r="L569" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M569" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -42708,7 +42892,7 @@
       </c>
       <c r="W569" t="inlineStr">
         <is>
-          <t>2026-01-28T03:44:51.539735</t>
+          <t>2026-01-28 23:15:51</t>
         </is>
       </c>
     </row>
@@ -44051,11 +44235,31 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H587" t="inlineStr"/>
-      <c r="I587" t="inlineStr"/>
-      <c r="J587" t="inlineStr"/>
-      <c r="K587" t="inlineStr"/>
-      <c r="L587" t="inlineStr"/>
+      <c r="H587" t="inlineStr">
+        <is>
+          <t>Southridge High School</t>
+        </is>
+      </c>
+      <c r="I587" t="inlineStr">
+        <is>
+          <t>Beaverton</t>
+        </is>
+      </c>
+      <c r="J587" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K587" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/hunter_sulte</t>
+        </is>
+      </c>
+      <c r="L587" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M587" t="inlineStr">
         <is>
           <t>Goalkeeper</t>
@@ -44090,7 +44294,7 @@
       </c>
       <c r="W587" t="inlineStr">
         <is>
-          <t>2026-01-28T03:46:30.020450</t>
+          <t>2026-01-28 23:18:55</t>
         </is>
       </c>
     </row>
@@ -44708,11 +44912,31 @@
           <t>California USA</t>
         </is>
       </c>
-      <c r="H596" t="inlineStr"/>
-      <c r="I596" t="inlineStr"/>
-      <c r="J596" t="inlineStr"/>
-      <c r="K596" t="inlineStr"/>
-      <c r="L596" t="inlineStr"/>
+      <c r="H596" t="inlineStr">
+        <is>
+          <t>Corner Canyon High School</t>
+        </is>
+      </c>
+      <c r="I596" t="inlineStr">
+        <is>
+          <t>Draper</t>
+        </is>
+      </c>
+      <c r="J596" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="K596" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/griffin_dillon</t>
+        </is>
+      </c>
+      <c r="L596" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M596" t="inlineStr">
         <is>
           <t>Midfielder</t>
@@ -44747,7 +44971,7 @@
       </c>
       <c r="W596" t="inlineStr">
         <is>
-          <t>2026-01-28T03:47:26.527136</t>
+          <t>2026-01-28 23:44:18</t>
         </is>
       </c>
     </row>
@@ -44980,7 +45204,7 @@
       </c>
       <c r="W599" t="inlineStr">
         <is>
-          <t>2026-01-28 11:23:48</t>
+          <t>2026-01-28 23:44:37</t>
         </is>
       </c>
     </row>
@@ -45308,11 +45532,23 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H604" t="inlineStr"/>
+      <c r="H604" t="inlineStr">
+        <is>
+          <t>Saratoga High School</t>
+        </is>
+      </c>
       <c r="I604" t="inlineStr"/>
       <c r="J604" t="inlineStr"/>
-      <c r="K604" t="inlineStr"/>
-      <c r="L604" t="inlineStr"/>
+      <c r="K604" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/sam_junqua</t>
+        </is>
+      </c>
+      <c r="L604" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M604" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -45347,7 +45583,7 @@
       </c>
       <c r="W604" t="inlineStr">
         <is>
-          <t>2026-01-28T03:48:08.934758</t>
+          <t>2026-01-28 23:45:37</t>
         </is>
       </c>
     </row>
@@ -54080,7 +54316,7 @@
       </c>
       <c r="W719" t="inlineStr">
         <is>
-          <t>2026-01-28T03:15:21.777457</t>
+          <t>2026-01-28 23:34:47</t>
         </is>
       </c>
     </row>
@@ -55014,11 +55250,23 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H732" t="inlineStr"/>
+      <c r="H732" t="inlineStr">
+        <is>
+          <t>Vista Ridge High School</t>
+        </is>
+      </c>
       <c r="I732" t="inlineStr"/>
       <c r="J732" t="inlineStr"/>
-      <c r="K732" t="inlineStr"/>
-      <c r="L732" t="inlineStr"/>
+      <c r="K732" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Khiry_Shelton</t>
+        </is>
+      </c>
+      <c r="L732" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M732" t="inlineStr">
         <is>
           <t>Forward</t>
@@ -55053,7 +55301,7 @@
       </c>
       <c r="W732" t="inlineStr">
         <is>
-          <t>2026-01-28T03:16:44.990005</t>
+          <t>2026-01-28 23:37:16</t>
         </is>
       </c>
     </row>
@@ -56003,11 +56251,23 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="H745" t="inlineStr"/>
+      <c r="H745" t="inlineStr">
+        <is>
+          <t>Columbia High School</t>
+        </is>
+      </c>
       <c r="I745" t="inlineStr"/>
       <c r="J745" t="inlineStr"/>
-      <c r="K745" t="inlineStr"/>
-      <c r="L745" t="inlineStr"/>
+      <c r="K745" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/caden_glover</t>
+        </is>
+      </c>
+      <c r="L745" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M745" t="inlineStr">
         <is>
           <t>Forward</t>
@@ -56036,7 +56296,7 @@
       </c>
       <c r="W745" t="inlineStr">
         <is>
-          <t>2026-01-28T03:58:59.195518</t>
+          <t>2026-01-28 23:39:40</t>
         </is>
       </c>
     </row>
@@ -57457,11 +57717,23 @@
           <t>Canada</t>
         </is>
       </c>
-      <c r="H765" t="inlineStr"/>
+      <c r="H765" t="inlineStr">
+        <is>
+          <t>St. Mary's High School</t>
+        </is>
+      </c>
       <c r="I765" t="inlineStr"/>
       <c r="J765" t="inlineStr"/>
-      <c r="K765" t="inlineStr"/>
-      <c r="L765" t="inlineStr"/>
+      <c r="K765" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/markus_cimermancic</t>
+        </is>
+      </c>
+      <c r="L765" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M765" t="inlineStr">
         <is>
           <t>Midfielder</t>
@@ -57490,7 +57762,7 @@
       </c>
       <c r="W765" t="inlineStr">
         <is>
-          <t>2026-01-28T04:00:50.801238</t>
+          <t>2026-01-28 23:24:48</t>
         </is>
       </c>
     </row>
@@ -57812,11 +58084,23 @@
           <t>Canada</t>
         </is>
       </c>
-      <c r="H770" t="inlineStr"/>
+      <c r="H770" t="inlineStr">
+        <is>
+          <t>Neil McNeil Catholic High School</t>
+        </is>
+      </c>
       <c r="I770" t="inlineStr"/>
       <c r="J770" t="inlineStr"/>
-      <c r="K770" t="inlineStr"/>
-      <c r="L770" t="inlineStr"/>
+      <c r="K770" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Kobe_Franklin</t>
+        </is>
+      </c>
+      <c r="L770" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M770" t="inlineStr">
         <is>
           <t>Defender</t>
@@ -57851,7 +58135,7 @@
       </c>
       <c r="W770" t="inlineStr">
         <is>
-          <t>2026-01-28T04:01:17.378412</t>
+          <t>2026-01-28 23:25:38</t>
         </is>
       </c>
     </row>
@@ -60871,11 +61155,23 @@
           <t>Japan</t>
         </is>
       </c>
-      <c r="H811" t="inlineStr"/>
+      <c r="H811" t="inlineStr">
+        <is>
+          <t>Kanagawa Prefectural Asahi High School</t>
+        </is>
+      </c>
       <c r="I811" t="inlineStr"/>
       <c r="J811" t="inlineStr"/>
-      <c r="K811" t="inlineStr"/>
-      <c r="L811" t="inlineStr"/>
+      <c r="K811" t="inlineStr">
+        <is>
+          <t>https://grokipedia.com/page/Yohei_Takaoka</t>
+        </is>
+      </c>
+      <c r="L811" t="inlineStr">
+        <is>
+          <t>Grokipedia</t>
+        </is>
+      </c>
       <c r="M811" t="inlineStr">
         <is>
           <t>Goalkeeper</t>
@@ -60910,7 +61206,7 @@
       </c>
       <c r="W811" t="inlineStr">
         <is>
-          <t>2026-01-28T04:05:02.313928</t>
+          <t>2026-01-28 23:32:51</t>
         </is>
       </c>
     </row>

</xml_diff>